<commit_message>
added plans for PWM module case
also added testing results, more pin assignments, and register
descriptions
</commit_message>
<xml_diff>
--- a/Software/Regiser Descriptions/Counter Mode Reg Description.xlsx
+++ b/Software/Regiser Descriptions/Counter Mode Reg Description.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="31">
   <si>
     <t>IP</t>
   </si>
@@ -76,6 +76,42 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>G1/G0 Read Mask</t>
+  </si>
+  <si>
+    <t>G1/G0 Write Mask</t>
+  </si>
+  <si>
+    <t>Motor CW</t>
+  </si>
+  <si>
+    <t>Motor CCW</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Wire Speed Home Switch</t>
+  </si>
+  <si>
+    <t>DIO[0] Register Description</t>
   </si>
 </sst>
 </file>
@@ -115,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -182,35 +218,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,16 +652,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="22" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="32" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="32" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
@@ -662,10 +773,10 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="12"/>
       <c r="E4">
         <v>0</v>
       </c>
@@ -687,137 +798,137 @@
       <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
       <c r="O4" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2" t="s">
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2" t="s">
+      <c r="W4" s="12"/>
+      <c r="X4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2" t="s">
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2" t="s">
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:34">
-      <c r="A5" s="3">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
         <v>1</v>
       </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6">
-        <v>0</v>
-      </c>
-      <c r="S5" s="6">
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="5">
         <v>1</v>
       </c>
-      <c r="T5" s="6">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5">
-        <v>0</v>
-      </c>
-      <c r="V5" s="4">
-        <v>0</v>
-      </c>
-      <c r="W5" s="5">
-        <v>0</v>
-      </c>
-      <c r="X5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="5" t="s">
+      <c r="T5" s="5">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Z5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="6">
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="5">
         <v>1</v>
       </c>
-      <c r="AB5" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="5">
+      <c r="AB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="4">
         <v>0</v>
       </c>
       <c r="AG5" t="s">
@@ -828,154 +939,154 @@
       </c>
     </row>
     <row r="6" spans="1:34">
-      <c r="A6" s="7">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7">
+      <c r="A6" s="11">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11">
         <v>6</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7">
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11">
         <v>8</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7">
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11">
         <v>2</v>
       </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7">
-        <v>0</v>
-      </c>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7">
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11">
+        <v>0</v>
+      </c>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11">
         <v>2</v>
       </c>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
       <c r="AG6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="16" thickBot="1"/>
     <row r="8" spans="1:34">
-      <c r="A8" s="3">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="6">
+      <c r="A8" s="2">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
         <v>1</v>
       </c>
-      <c r="R8" s="6">
-        <v>0</v>
-      </c>
-      <c r="S8" s="6">
-        <v>0</v>
-      </c>
-      <c r="T8" s="6">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5">
-        <v>0</v>
-      </c>
-      <c r="V8" s="4">
-        <v>0</v>
-      </c>
-      <c r="W8" s="5">
-        <v>0</v>
-      </c>
-      <c r="X8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="4">
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
         <v>1</v>
       </c>
-      <c r="AD8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="6">
+      <c r="AD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="5">
         <v>1</v>
       </c>
-      <c r="AF8" s="5">
+      <c r="AF8" s="4">
         <v>0</v>
       </c>
       <c r="AG8" t="s">
@@ -986,60 +1097,707 @@
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="7">
-        <v>0</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7">
-        <v>0</v>
-      </c>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7">
+      <c r="A9" s="11">
+        <v>0</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11">
         <v>8</v>
       </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7">
-        <v>0</v>
-      </c>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7" t="s">
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11">
+        <v>0</v>
+      </c>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="7"/>
-      <c r="AE9" s="7"/>
-      <c r="AF9" s="7"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
       <c r="AG9" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:34">
+      <c r="A15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="6">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6">
+        <v>30</v>
+      </c>
+      <c r="C17" s="6">
+        <v>29</v>
+      </c>
+      <c r="D17" s="6">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6">
+        <v>26</v>
+      </c>
+      <c r="G17" s="6">
+        <v>25</v>
+      </c>
+      <c r="H17" s="6">
+        <v>24</v>
+      </c>
+      <c r="I17" s="6">
+        <v>23</v>
+      </c>
+      <c r="J17" s="6">
+        <v>22</v>
+      </c>
+      <c r="K17" s="6">
+        <v>21</v>
+      </c>
+      <c r="L17" s="6">
+        <v>20</v>
+      </c>
+      <c r="M17" s="6">
+        <v>19</v>
+      </c>
+      <c r="N17" s="6">
+        <v>18</v>
+      </c>
+      <c r="O17" s="6">
+        <v>17</v>
+      </c>
+      <c r="P17" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="6">
+        <v>15</v>
+      </c>
+      <c r="R17" s="6">
+        <v>14</v>
+      </c>
+      <c r="S17" s="6">
+        <v>13</v>
+      </c>
+      <c r="T17" s="6">
+        <v>12</v>
+      </c>
+      <c r="U17" s="6">
+        <v>11</v>
+      </c>
+      <c r="V17" s="6">
+        <v>10</v>
+      </c>
+      <c r="W17" s="6">
+        <v>9</v>
+      </c>
+      <c r="X17" s="6">
+        <v>8</v>
+      </c>
+      <c r="Y17" s="6">
+        <v>7</v>
+      </c>
+      <c r="Z17" s="6">
+        <v>6</v>
+      </c>
+      <c r="AA17" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB17" s="6">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="6">
+        <v>3</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="7">
+        <v>23</v>
+      </c>
+      <c r="J18" s="7">
+        <v>22</v>
+      </c>
+      <c r="K18" s="7">
+        <v>21</v>
+      </c>
+      <c r="L18" s="7">
+        <v>20</v>
+      </c>
+      <c r="M18" s="6">
+        <v>19</v>
+      </c>
+      <c r="N18" s="6">
+        <v>18</v>
+      </c>
+      <c r="O18" s="6">
+        <v>17</v>
+      </c>
+      <c r="P18" s="6">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>15</v>
+      </c>
+      <c r="R18" s="6">
+        <v>14</v>
+      </c>
+      <c r="S18" s="6">
+        <v>13</v>
+      </c>
+      <c r="T18" s="6">
+        <v>12</v>
+      </c>
+      <c r="U18" s="6">
+        <v>11</v>
+      </c>
+      <c r="V18" s="6">
+        <v>10</v>
+      </c>
+      <c r="W18" s="6">
+        <v>9</v>
+      </c>
+      <c r="X18" s="6">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>7</v>
+      </c>
+      <c r="Z18" s="6">
+        <v>6</v>
+      </c>
+      <c r="AA18" s="6">
+        <v>5</v>
+      </c>
+      <c r="AB18" s="6">
+        <v>4</v>
+      </c>
+      <c r="AC18" s="6">
+        <v>3</v>
+      </c>
+      <c r="AD18" s="6">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="7">
+        <v>1</v>
+      </c>
+      <c r="J19" s="7">
+        <v>3</v>
+      </c>
+      <c r="K19" s="7">
+        <v>5</v>
+      </c>
+      <c r="L19" s="7">
+        <v>7</v>
+      </c>
+      <c r="M19" s="7">
+        <v>9</v>
+      </c>
+      <c r="N19" s="7">
+        <v>11</v>
+      </c>
+      <c r="O19" s="7">
+        <v>13</v>
+      </c>
+      <c r="P19" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>17</v>
+      </c>
+      <c r="R19" s="7">
+        <v>19</v>
+      </c>
+      <c r="S19" s="7">
+        <v>21</v>
+      </c>
+      <c r="T19" s="7">
+        <v>23</v>
+      </c>
+      <c r="U19" s="7">
+        <v>25</v>
+      </c>
+      <c r="V19" s="7">
+        <v>27</v>
+      </c>
+      <c r="W19" s="7">
+        <v>29</v>
+      </c>
+      <c r="X19" s="7">
+        <v>31</v>
+      </c>
+      <c r="Y19" s="7">
+        <v>33</v>
+      </c>
+      <c r="Z19" s="7">
+        <v>35</v>
+      </c>
+      <c r="AA19" s="7">
+        <v>37</v>
+      </c>
+      <c r="AB19" s="7">
+        <v>39</v>
+      </c>
+      <c r="AC19" s="7">
+        <v>41</v>
+      </c>
+      <c r="AD19" s="7">
+        <v>43</v>
+      </c>
+      <c r="AE19" s="7">
+        <v>45</v>
+      </c>
+      <c r="AF19" s="7">
+        <v>47</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="I20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="I21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11">
+        <v>3</v>
+      </c>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="I22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="9">
+        <v>1</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="I23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="I24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="9">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="W24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="X24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="36">
+    <mergeCell ref="AC21:AF21"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="Q21:T21"/>
+    <mergeCell ref="U21:X21"/>
+    <mergeCell ref="Y21:AB21"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="AC20:AF20"/>
+    <mergeCell ref="Y20:AB20"/>
+    <mergeCell ref="U20:X20"/>
+    <mergeCell ref="Q20:T20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="U6:X6"/>
     <mergeCell ref="Y6:AB6"/>
     <mergeCell ref="AC6:AF6"/>
@@ -1056,13 +1814,6 @@
     <mergeCell ref="I6:L6"/>
     <mergeCell ref="M6:P6"/>
     <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AB4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>